<commit_message>
Some quality of life fixes
</commit_message>
<xml_diff>
--- a/Recipients data.xlsx
+++ b/Recipients data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B85612-EAF1-43EB-A47C-EC25301596E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2280" yWindow="0" windowWidth="15280" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipients" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Message</t>
   </si>
@@ -22,28 +23,22 @@
     <t>Username</t>
   </si>
   <si>
-    <t>Hi ** Important Text **: Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book.</t>
+    <t>@pigeon12</t>
   </si>
   <si>
-    <t>@local_bot</t>
-  </si>
-  <si>
-    <t>@publicbot</t>
-  </si>
-  <si>
-    <t>@Enjin_Airdrop_bot</t>
-  </si>
-  <si>
-    <t>@thelazy_bot</t>
-  </si>
-  <si>
-    <t>@ArtiBot</t>
+    <t>ПРИМЕР СКРИПТА
+Здравствуй! Меня зовут Серафим, я представляю международную организацию AIESEC💫
+В этом году ты принимал(а) участие в онлайн-форуме YouLead’22.
+В опросе ты указал(а), что тебе было бы интересно послушать о социальных проектах, которые будут проходить в ближайшее время по всей России! И вот как раз уже очень скоро начнётся их реализация, которые направлены на разные цели устойчивого развития🤍
+Хотел бы ты узнать об этом побольше? Я готов(а) ответить на все твои вопросы! 
+Ссылка на регистрацию на проекты от AIESEC: http://aiesec.finek.tilda.ws/projects
+(это сообщение было отправлено с помощью кода, написанного на Python, мне было лень отправлять сообщения каждому по отдельности, но в итоге его написание заняло ещё больше времени... (ㅠ﹏ㅠ)  )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,15 +48,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -69,11 +70,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -81,16 +97,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -114,27 +141,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Message" displayName="Message" ref="C1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="1">
-    <tableColumn id="1" name="Username"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Message" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C1:C3" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F85B5A9A-3A56-400D-82B4-99C934AE5BCD}" name="Username" displayName="Username" ref="A1:A6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:A6" xr:uid="{F85B5A9A-3A56-400D-82B4-99C934AE5BCD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Message" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{DECCA338-2F83-4CAE-950E-2DCE49EAD81F}" name="Username" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -172,7 +200,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -207,6 +235,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -242,9 +287,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,22 +479,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="92.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="115.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1"/>
@@ -440,36 +502,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some quality of life fixes 2.0
</commit_message>
<xml_diff>
--- a/Recipients data.xlsx
+++ b/Recipients data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B85612-EAF1-43EB-A47C-EC25301596E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA69E9E-F55D-4F16-81D0-ED2DAB9FEE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="0" windowWidth="15280" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Message</t>
   </si>
@@ -23,23 +23,43 @@
     <t>Username</t>
   </si>
   <si>
-    <t>@pigeon12</t>
-  </si>
-  <si>
-    <t>ПРИМЕР СКРИПТА
-Здравствуй! Меня зовут Серафим, я представляю международную организацию AIESEC💫
+    <t>Виктор Лазарев</t>
+  </si>
+  <si>
+    <t>89110392394(по номеру)</t>
+  </si>
+  <si>
+    <t>EveeeInn</t>
+  </si>
+  <si>
+    <t>Valeriya Petryakova</t>
+  </si>
+  <si>
+    <t>Vmaslovva</t>
+  </si>
+  <si>
+    <t>Zzzzz</t>
+  </si>
+  <si>
+    <t>Столбец1</t>
+  </si>
+  <si>
+    <t>Здравствуй! Меня зовут Серафим, я представляю международную организацию AIESEC💫
 В этом году ты принимал(а) участие в онлайн-форуме YouLead’22.
 В опросе ты указал(а), что тебе было бы интересно послушать о социальных проектах, которые будут проходить в ближайшее время по всей России! И вот как раз уже очень скоро начнётся их реализация, которые направлены на разные цели устойчивого развития🤍
 Хотел бы ты узнать об этом побольше? Я готов(а) ответить на все твои вопросы! 
 Ссылка на регистрацию на проекты от AIESEC: http://aiesec.finek.tilda.ws/projects
 (это сообщение было отправлено с помощью кода, написанного на Python, мне было лень отправлять сообщения каждому по отдельности, но в итоге его написание заняло ещё больше времени... (ㅠ﹏ㅠ)  )</t>
   </si>
+  <si>
+    <t>@m4y31x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,8 +67,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,8 +96,26 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF34A853"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -71,25 +124,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
       </left>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
       </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,19 +180,54 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -141,19 +258,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Message" displayName="Message" ref="C1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Message" displayName="Message" ref="C1:C9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Message" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Message" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F85B5A9A-3A56-400D-82B4-99C934AE5BCD}" name="Username" displayName="Username" ref="A1:A6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:A6" xr:uid="{F85B5A9A-3A56-400D-82B4-99C934AE5BCD}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DECCA338-2F83-4CAE-950E-2DCE49EAD81F}" name="Username" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F85B5A9A-3A56-400D-82B4-99C934AE5BCD}" name="Username" displayName="Username" ref="A1:B40" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B40" xr:uid="{F85B5A9A-3A56-400D-82B4-99C934AE5BCD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DECCA338-2F83-4CAE-950E-2DCE49EAD81F}" name="Username" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{AF934D03-628D-4247-BE05-D4238D4A43D6}" name="Столбец1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -480,9 +598,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -493,65 +611,160 @@
     <col min="3" max="3" width="115.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1"/>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14"/>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="5"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B3"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B5"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18"/>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="9">
+        <v>89825550678</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="10"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="11">
+        <v>89515709459</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="6"/>
+    </row>
+    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="6"/>
+    </row>
+    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="12"/>
+    </row>
+    <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="6"/>
+    </row>
+    <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="6"/>
+    </row>
+    <row r="37" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="12"/>
+    </row>
+    <row r="39" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>